<commit_message>
Rerun with corrected electricity cost
</commit_message>
<xml_diff>
--- a/input_files/case_files/BTES_base_case.xlsx
+++ b/input_files/case_files/BTES_base_case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/m_/v6c97p3x1mg6bmvchddj43dc0000gn/T/fz3temp-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BD2979-99F8-344B-A5EA-05E1C16015AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDED8AA3-AFEE-724E-83AA-DC0297FE7263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,9 +98,6 @@
     <t>Note that for MEM, storage is in energy units whereas for PyPSA it is in power units.</t>
   </si>
   <si>
-    <t>nuclear</t>
-  </si>
-  <si>
     <t>wind</t>
   </si>
   <si>
@@ -369,6 +366,9 @@
   </si>
   <si>
     <t>btes_base_case_orca</t>
+  </si>
+  <si>
+    <t>Lithium-Ion-LFP-bicharger % discharge</t>
   </si>
 </sst>
 </file>
@@ -1263,8 +1263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1289,7 +1289,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1307,7 +1307,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1345,7 +1345,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1376,7 +1376,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1388,7 +1388,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1400,7 +1400,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1427,10 +1427,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1442,7 +1442,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1454,7 +1454,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1466,7 +1466,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1475,10 +1475,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1490,7 +1490,7 @@
         <v>8</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1502,7 +1502,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1516,18 +1516,18 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1535,7 +1535,7 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1543,41 +1543,41 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C31" s="6"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -1586,19 +1586,19 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B33" s="11">
         <f>((B31-B30)*24+1)/B32</f>
         <v>8760.0000000000582</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B34" s="11">
         <f>B33*B32</f>
@@ -1611,23 +1611,23 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>76</v>
       </c>
       <c r="C36" s="4"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
@@ -1639,39 +1639,39 @@
       </c>
       <c r="C38" s="1"/>
       <c r="D38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C40" s="1"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C42" s="1"/>
     </row>
@@ -1679,7 +1679,7 @@
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="F43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
@@ -1687,23 +1687,23 @@
         <v>9</v>
       </c>
       <c r="I44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:22" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
@@ -1714,22 +1714,22 @@
         <v>12</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G49" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H49" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>14</v>
@@ -1738,18 +1738,18 @@
         <v>15</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N49" s="2" t="s">
         <v>8</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B50" t="s">
         <v>10</v>
@@ -1758,10 +1758,10 @@
         <v>10</v>
       </c>
       <c r="D50" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G50" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I50" s="5"/>
       <c r="K50" s="5"/>
@@ -1770,320 +1770,322 @@
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C51" t="s">
         <v>18</v>
       </c>
       <c r="D51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I51" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J51" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L51" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
       <c r="N51" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O51" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C52" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H52" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I52" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J52" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L52" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
       <c r="N52" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O52" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B53" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="C53" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D53" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I53" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J53" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L53" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
       <c r="N53" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O53" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B54" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C54" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="D54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I54" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J54" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L54" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
       <c r="N54" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O54" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A55" s="6" t="s">
-        <v>36</v>
+      <c r="A55" t="s">
+        <v>63</v>
       </c>
       <c r="B55" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C55" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="D55" t="s">
+        <v>90</v>
+      </c>
+      <c r="E55" t="s">
         <v>91</v>
       </c>
-      <c r="I55" s="15" t="s">
-        <v>83</v>
+      <c r="I55" s="5" t="s">
+        <v>82</v>
       </c>
       <c r="J55" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L55" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
       <c r="N55" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O55" s="5" t="s">
-        <v>83</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="R55" s="5"/>
+      <c r="V55" s="5"/>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>64</v>
       </c>
       <c r="B56" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C56" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D56" t="s">
         <v>91</v>
       </c>
-      <c r="E56" t="s">
-        <v>92</v>
-      </c>
-      <c r="F56">
-        <v>-1</v>
-      </c>
       <c r="I56" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J56" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="K56" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L56" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
+      <c r="M56" t="b">
+        <v>1</v>
+      </c>
       <c r="N56" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O56" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R56" s="5"/>
       <c r="V56" s="5"/>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B57" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="C57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D57" t="s">
-        <v>92</v>
-      </c>
-      <c r="I57" s="5" t="s">
-        <v>83</v>
+        <v>91</v>
+      </c>
+      <c r="E57" t="s">
+        <v>90</v>
+      </c>
+      <c r="I57" s="5">
+        <v>0</v>
       </c>
       <c r="J57" t="str">
-        <f>B42 &amp; "/time range/" &amp; B41</f>
-        <v>$/time range/MW</v>
+        <f>B41 &amp; "/time range/" &amp; B40</f>
+        <v>MW/time range/h</v>
       </c>
       <c r="K57" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L57" t="str">
-        <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
-        <v>$/MWh</v>
-      </c>
-      <c r="M57" t="b">
-        <v>1</v>
+        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
+        <v>MW/h</v>
       </c>
       <c r="N57" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O57" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R57" s="5"/>
       <c r="V57" s="5"/>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B58" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C58" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D58" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E58" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I58" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J58" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="K58" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L58" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
       <c r="N58" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O58" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B59" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C59" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D59" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I59" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J59" t="str">
         <f>B42 &amp; "/time range/" &amp; B41 &amp; B40</f>
         <v>$/time range/MWh</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L59" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
@@ -2093,109 +2095,109 @@
         <v>1</v>
       </c>
       <c r="N59" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O59" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P59" s="1"/>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B60" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C60" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D60" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E60" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I60" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J60" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L60" s="13" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
       <c r="N60" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O60" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C61" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D61" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E61" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I61" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J61" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L61" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
       <c r="N61" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O61" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B62" t="s">
+        <v>86</v>
+      </c>
+      <c r="C62" t="s">
+        <v>85</v>
+      </c>
+      <c r="D62" t="s">
         <v>87</v>
       </c>
-      <c r="C62" t="s">
-        <v>86</v>
-      </c>
-      <c r="D62" t="s">
-        <v>88</v>
-      </c>
       <c r="I62" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J62" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="K62" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L62" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
@@ -2205,58 +2207,58 @@
         <v>1</v>
       </c>
       <c r="N62" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O62" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C63" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D63" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E63" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I63" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J63" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="K63" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L63" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
       <c r="N63" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O63" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B64" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D64" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I64" s="15"/>
       <c r="K64" s="5">
@@ -2271,12 +2273,12 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
@@ -2286,7 +2288,7 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
@@ -2295,7 +2297,7 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L71" s="7"/>
       <c r="M71" s="7"/>

</xml_diff>

<commit_message>
Update repo before submission
</commit_message>
<xml_diff>
--- a/input_files/case_files/BTES_base_case.xlsx
+++ b/input_files/case_files/BTES_base_case.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/mb/bhrh7_m94j739pkhyn5p1l3w0000gn/T/fz3temp-2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awongel/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3189BA4-FE4B-2B4E-8362-71B8C0BE3205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A39BCFA-0071-6C40-89B0-68F680FE9D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -251,9 +251,6 @@
     <t>costs_path</t>
   </si>
   <si>
-    <t>p_min_pu</t>
-  </si>
-  <si>
     <t>Note: p_min_pu allow bidirectionality of link</t>
   </si>
   <si>
@@ -344,21 +341,6 @@
     <t>lost_load</t>
   </si>
   <si>
-    <t>CONUS_demand_2015_2024.csv</t>
-  </si>
-  <si>
-    <t>2019-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2019-12-31 23:00:00</t>
-  </si>
-  <si>
-    <t>CONUS_solar_CF_2019.csv</t>
-  </si>
-  <si>
-    <t>CONUS_wind_CF_2019.csv</t>
-  </si>
-  <si>
     <t>battery</t>
   </si>
   <si>
@@ -369,6 +351,24 @@
   </si>
   <si>
     <t>Lithium-Ion-LFP-bicharger % discharge</t>
+  </si>
+  <si>
+    <t>CONUS_demand_2019_2023.csv</t>
+  </si>
+  <si>
+    <t>CONUS_solar_CF_2019_2023.csv</t>
+  </si>
+  <si>
+    <t>CONUS_wind_CF_2019_2023.csv</t>
+  </si>
+  <si>
+    <t>p_nom_min</t>
+  </si>
+  <si>
+    <t>2020-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2023-12-31 23:00:00</t>
   </si>
 </sst>
 </file>
@@ -1263,8 +1263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1519,7 +1519,7 @@
         <v>30</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1527,7 +1527,7 @@
         <v>71</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1543,7 +1543,7 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1551,7 +1551,7 @@
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1559,7 +1559,7 @@
         <v>27</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" t="s">
@@ -1571,7 +1571,7 @@
         <v>28</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C31" s="6"/>
     </row>
@@ -1590,7 +1590,7 @@
       </c>
       <c r="B33" s="11">
         <f>((B31-B30)*24+1)/B32</f>
-        <v>8760.0000000000582</v>
+        <v>35064.000000000058</v>
       </c>
       <c r="C33" t="s">
         <v>65</v>
@@ -1602,7 +1602,7 @@
       </c>
       <c r="B34" s="11">
         <f>B33*B32</f>
-        <v>8760.0000000000582</v>
+        <v>35064.000000000058</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
@@ -1611,10 +1611,10 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="14" t="s">
         <v>74</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>75</v>
       </c>
       <c r="C36" s="4"/>
     </row>
@@ -1623,7 +1623,7 @@
         <v>33</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" t="s">
@@ -1645,7 +1645,7 @@
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
@@ -1659,10 +1659,10 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C41" s="1"/>
     </row>
@@ -1679,7 +1679,7 @@
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="F43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
@@ -1723,13 +1723,13 @@
         <v>24</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="G49" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H49" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>14</v>
@@ -1744,7 +1744,7 @@
         <v>8</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.2">
@@ -1758,10 +1758,10 @@
         <v>10</v>
       </c>
       <c r="D50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G50" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I50" s="5"/>
       <c r="K50" s="5"/>
@@ -1773,36 +1773,36 @@
         <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C51" t="s">
         <v>18</v>
       </c>
       <c r="D51" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H51" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I51" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J51" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L51" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
       <c r="N51" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O51" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.2">
@@ -1810,36 +1810,36 @@
         <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C52" t="s">
         <v>21</v>
       </c>
       <c r="D52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H52" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I52" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J52" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L52" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
       <c r="N52" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O52" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.2">
@@ -1847,33 +1847,33 @@
         <v>35</v>
       </c>
       <c r="B53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C53" t="s">
         <v>19</v>
       </c>
       <c r="D53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I53" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J53" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L53" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
       <c r="N53" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O53" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.2">
@@ -1881,33 +1881,33 @@
         <v>35</v>
       </c>
       <c r="B54" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C54" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I54" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J54" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L54" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
       <c r="N54" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O54" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.2">
@@ -1915,36 +1915,36 @@
         <v>63</v>
       </c>
       <c r="B55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C55" t="s">
+        <v>102</v>
+      </c>
+      <c r="D55" t="s">
         <v>89</v>
       </c>
-      <c r="C55" t="s">
-        <v>108</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>90</v>
       </c>
-      <c r="E55" t="s">
-        <v>91</v>
-      </c>
       <c r="I55" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J55" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L55" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
       <c r="N55" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O55" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="R55" s="5"/>
       <c r="V55" s="5"/>
@@ -1954,23 +1954,23 @@
         <v>64</v>
       </c>
       <c r="B56" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C56" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D56" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J56" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="K56" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L56" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
@@ -1980,10 +1980,10 @@
         <v>1</v>
       </c>
       <c r="N56" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O56" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="R56" s="5"/>
       <c r="V56" s="5"/>
@@ -1993,16 +1993,16 @@
         <v>63</v>
       </c>
       <c r="B57" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C57" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D57" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E57" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I57" s="5">
         <v>0</v>
@@ -2012,17 +2012,17 @@
         <v>MW/time range/h</v>
       </c>
       <c r="K57" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L57" t="str">
         <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
         <v>MW/h</v>
       </c>
       <c r="N57" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O57" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="R57" s="5"/>
       <c r="V57" s="5"/>
@@ -2035,33 +2035,33 @@
         <v>23</v>
       </c>
       <c r="C58" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D58" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E58" t="s">
         <v>25</v>
       </c>
       <c r="I58" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J58" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="K58" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L58" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
       <c r="N58" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O58" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.2">
@@ -2069,23 +2069,23 @@
         <v>64</v>
       </c>
       <c r="B59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C59" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D59" t="s">
         <v>25</v>
       </c>
       <c r="I59" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J59" t="str">
         <f>B42 &amp; "/time range/" &amp; B41 &amp; B40</f>
         <v>$/time range/MWh</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L59" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
@@ -2095,10 +2095,10 @@
         <v>1</v>
       </c>
       <c r="N59" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O59" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P59" s="1"/>
     </row>
@@ -2107,36 +2107,36 @@
         <v>63</v>
       </c>
       <c r="B60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C60" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D60" t="s">
         <v>25</v>
       </c>
       <c r="E60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I60" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J60" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L60" s="13" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
       <c r="N60" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O60" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.2">
@@ -2144,36 +2144,36 @@
         <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C61" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D61" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E61" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I61" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J61" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L61" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
       <c r="N61" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O61" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.2">
@@ -2181,23 +2181,23 @@
         <v>64</v>
       </c>
       <c r="B62" t="s">
+        <v>85</v>
+      </c>
+      <c r="C62" t="s">
+        <v>84</v>
+      </c>
+      <c r="D62" t="s">
         <v>86</v>
       </c>
-      <c r="C62" t="s">
-        <v>85</v>
-      </c>
-      <c r="D62" t="s">
-        <v>87</v>
-      </c>
       <c r="I62" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J62" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="K62" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L62" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
@@ -2207,10 +2207,10 @@
         <v>1</v>
       </c>
       <c r="N62" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O62" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.2">
@@ -2218,36 +2218,36 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C63" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D63" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E63" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I63" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J63" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="K63" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L63" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
       <c r="N63" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O63" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.2">
@@ -2255,10 +2255,10 @@
         <v>35</v>
       </c>
       <c r="B64" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D64" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I64" s="15"/>
       <c r="K64" s="5">
@@ -2279,6 +2279,9 @@
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>32</v>
+      </c>
+      <c r="F68">
+        <v>566000</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>